<commit_message>
Functioanality was moved to class::Roo::Excelx::Sheet
</commit_message>
<xml_diff>
--- a/spec/fixtures/bar.xlsx
+++ b/spec/fixtures/bar.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MEN'S" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -496,15 +497,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>511200</xdr:colOff>
+      <xdr:colOff>538200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>959760</xdr:rowOff>
+      <xdr:rowOff>950760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>967680</xdr:colOff>
+      <xdr:colOff>994320</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>930600</xdr:rowOff>
+      <xdr:rowOff>921240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -519,8 +520,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1443960" y="2331360"/>
-          <a:ext cx="456480" cy="948600"/>
+          <a:off x="1470960" y="2322360"/>
+          <a:ext cx="456120" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -535,15 +536,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>320760</xdr:colOff>
+      <xdr:colOff>347760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>388080</xdr:rowOff>
+      <xdr:rowOff>379080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
+      <xdr:colOff>37440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>932400</xdr:rowOff>
+      <xdr:rowOff>923040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -558,8 +559,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1253520" y="388080"/>
-          <a:ext cx="888120" cy="937800"/>
+          <a:off x="1280520" y="379080"/>
+          <a:ext cx="887760" cy="937440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,15 +575,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>360360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>963720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:colOff>1159560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>880560</xdr:rowOff>
+      <xdr:rowOff>871200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -597,8 +598,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1266120" y="3322080"/>
-          <a:ext cx="799560" cy="873000"/>
+          <a:off x="1293120" y="3313080"/>
+          <a:ext cx="799200" cy="872640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -613,15 +614,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>525600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>955080</xdr:colOff>
+      <xdr:colOff>981720</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>937440</xdr:rowOff>
+      <xdr:rowOff>928080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -636,8 +637,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1431360" y="6192360"/>
-          <a:ext cx="456480" cy="917280"/>
+          <a:off x="1458360" y="6183360"/>
+          <a:ext cx="456120" cy="916920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -652,15 +653,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>193680</xdr:colOff>
+      <xdr:colOff>220680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>972720</xdr:rowOff>
+      <xdr:rowOff>963720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>50760</xdr:colOff>
+      <xdr:colOff>77400</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1086120</xdr:rowOff>
+      <xdr:rowOff>1076760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -675,8 +676,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1126440" y="9100440"/>
-          <a:ext cx="1055160" cy="1091520"/>
+          <a:off x="1153440" y="9091440"/>
+          <a:ext cx="1054800" cy="1091160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -691,15 +692,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>460440</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>487440</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>976320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>929520</xdr:colOff>
+      <xdr:colOff>956160</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>912960</xdr:rowOff>
+      <xdr:rowOff>903600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -714,8 +715,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1393200" y="7157520"/>
-          <a:ext cx="469080" cy="905400"/>
+          <a:off x="1420200" y="7148520"/>
+          <a:ext cx="468720" cy="905040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -730,15 +731,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>231840</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>258840</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1167120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>21600</xdr:colOff>
+      <xdr:colOff>48240</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1099080</xdr:rowOff>
+      <xdr:rowOff>1089720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -753,8 +754,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1164600" y="12593160"/>
-          <a:ext cx="987840" cy="1091520"/>
+          <a:off x="1191600" y="12584160"/>
+          <a:ext cx="987480" cy="1091160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -769,15 +770,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>168480</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>195480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1128960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>124560</xdr:colOff>
+      <xdr:colOff>151200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1086480</xdr:rowOff>
+      <xdr:rowOff>1077120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -792,8 +793,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1101240" y="13723560"/>
-          <a:ext cx="1154160" cy="1078920"/>
+          <a:off x="1128240" y="13714560"/>
+          <a:ext cx="1153800" cy="1078560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -808,15 +809,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>308160</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>972720</xdr:rowOff>
+      <xdr:rowOff>963720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1171080</xdr:colOff>
+      <xdr:colOff>1197720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>946080</xdr:rowOff>
+      <xdr:rowOff>936720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -831,8 +832,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1240920" y="1366200"/>
-          <a:ext cx="862920" cy="951480"/>
+          <a:off x="1267920" y="1357200"/>
+          <a:ext cx="862560" cy="951120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,15 +848,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>460440</xdr:colOff>
+      <xdr:colOff>487440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>972360</xdr:rowOff>
+      <xdr:rowOff>963360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>934200</xdr:colOff>
+      <xdr:colOff>960840</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>933840</xdr:rowOff>
+      <xdr:rowOff>924480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,8 +871,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1393200" y="8122320"/>
-          <a:ext cx="473760" cy="939240"/>
+          <a:off x="1420200" y="8113320"/>
+          <a:ext cx="473400" cy="938880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,15 +887,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>523800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>550800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1103400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1031040</xdr:colOff>
+      <xdr:colOff>1057680</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1095840</xdr:rowOff>
+      <xdr:rowOff>1086480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -909,8 +910,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1456560" y="15971400"/>
-          <a:ext cx="507240" cy="1088280"/>
+          <a:off x="1483560" y="15962400"/>
+          <a:ext cx="506880" cy="1087920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -925,15 +926,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333360</xdr:colOff>
+      <xdr:colOff>360360</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1124640</xdr:rowOff>
+      <xdr:rowOff>1115640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1190520</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1187640</xdr:rowOff>
+      <xdr:rowOff>1178280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -948,8 +949,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1266120" y="17088480"/>
-          <a:ext cx="857160" cy="1193040"/>
+          <a:off x="1293120" y="17079480"/>
+          <a:ext cx="856800" cy="1192680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -964,15 +965,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>536760</xdr:colOff>
+      <xdr:colOff>563760</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>947160</xdr:rowOff>
+      <xdr:rowOff>938160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>979200</xdr:colOff>
+      <xdr:colOff>1005840</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>920880</xdr:rowOff>
+      <xdr:rowOff>911520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -987,8 +988,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1469520" y="5214240"/>
-          <a:ext cx="442440" cy="926280"/>
+          <a:off x="1496520" y="5205240"/>
+          <a:ext cx="442080" cy="925920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1003,15 +1004,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>511200</xdr:colOff>
+      <xdr:colOff>538200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1150200</xdr:rowOff>
+      <xdr:rowOff>1141200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1018440</xdr:colOff>
+      <xdr:colOff>1045080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1124280</xdr:rowOff>
+      <xdr:rowOff>1114920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1026,8 +1027,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1443960" y="11399040"/>
-          <a:ext cx="507240" cy="1142280"/>
+          <a:off x="1470960" y="11390040"/>
+          <a:ext cx="506880" cy="1141920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,15 +1043,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>447840</xdr:colOff>
+      <xdr:colOff>474840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1137600</xdr:rowOff>
+      <xdr:rowOff>1128600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1031400</xdr:colOff>
+      <xdr:colOff>1058040</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1108800</xdr:rowOff>
+      <xdr:rowOff>1099440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1065,8 +1066,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1380600" y="10243440"/>
-          <a:ext cx="583560" cy="1114200"/>
+          <a:off x="1407600" y="10234440"/>
+          <a:ext cx="583200" cy="1113840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1081,15 +1082,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>308160</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1069560</xdr:colOff>
+      <xdr:colOff>1096200</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1106640</xdr:rowOff>
+      <xdr:rowOff>1097280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1104,8 +1105,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1240920" y="19438200"/>
-          <a:ext cx="761400" cy="1086480"/>
+          <a:off x="1267920" y="19429200"/>
+          <a:ext cx="761040" cy="1086120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1120,15 +1121,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>345960</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>372960</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>951120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1145520</xdr:colOff>
+      <xdr:colOff>1172160</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>901440</xdr:rowOff>
+      <xdr:rowOff>892080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1143,8 +1144,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1278720" y="4274640"/>
-          <a:ext cx="799560" cy="893880"/>
+          <a:off x="1305720" y="4265640"/>
+          <a:ext cx="799200" cy="893520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1159,15 +1160,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>308160</xdr:colOff>
+      <xdr:colOff>335160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>91800</xdr:colOff>
+      <xdr:colOff>118440</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>933840</xdr:rowOff>
+      <xdr:rowOff>924480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1182,8 +1183,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1240920" y="18384120"/>
-          <a:ext cx="981720" cy="862920"/>
+          <a:off x="1267920" y="18375120"/>
+          <a:ext cx="981360" cy="862560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1198,15 +1199,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>358920</xdr:colOff>
+      <xdr:colOff>385920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1114200</xdr:colOff>
+      <xdr:colOff>1140840</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>997200</xdr:rowOff>
+      <xdr:rowOff>987840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1221,8 +1222,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1291680" y="14879160"/>
-          <a:ext cx="755280" cy="977040"/>
+          <a:off x="1318680" y="14870160"/>
+          <a:ext cx="754920" cy="976680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1244,7 +1245,7 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -2272,4 +2273,27 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>